<commit_message>
adding the Payroll staff record
</commit_message>
<xml_diff>
--- a/bin/config/ePaymentConnector.xlsx
+++ b/bin/config/ePaymentConnector.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12705" windowHeight="2100" tabRatio="710" firstSheet="21" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12030" windowHeight="2100" tabRatio="710" firstSheet="22" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="UploadSalariesPensionTest" sheetId="23" r:id="rId22"/>
     <sheet name="LogoutTest" sheetId="8" r:id="rId23"/>
     <sheet name="BankBranchSetupTest" sheetId="31" r:id="rId24"/>
+    <sheet name="ManageStaffRecordTest" sheetId="32" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K5"/>
+  <oleSize ref="A1:L5"/>
 </workbook>
 </file>
 
@@ -1872,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2018,6 +2019,18 @@
     <hyperlink ref="J2" r:id="rId1"/>
     <hyperlink ref="R2" r:id="rId2"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
latest edition before upgrade of laptop
</commit_message>
<xml_diff>
--- a/bin/config/ePaymentConnector.xlsx
+++ b/bin/config/ePaymentConnector.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12345" windowHeight="1800" tabRatio="710" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11220" windowHeight="3900" tabRatio="710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -43,14 +43,21 @@
     <sheet name="StandingOrderDateTest" sheetId="40" r:id="rId34"/>
     <sheet name="StandingOrderOthersTest" sheetId="41" r:id="rId35"/>
     <sheet name="PaySalaryViaRRRTest" sheetId="42" r:id="rId36"/>
+    <sheet name="PayVendorsAndSuppliersTest" sheetId="45" r:id="rId37"/>
+    <sheet name="PayTaxesRRRTest" sheetId="46" r:id="rId38"/>
+    <sheet name="PayPensionViaRRRTest" sheetId="47" r:id="rId39"/>
+    <sheet name="PayRegisteredBillerTellerTest" sheetId="48" r:id="rId40"/>
+    <sheet name="StandingOrderDateTest01" sheetId="49" r:id="rId41"/>
+    <sheet name="StandingOrderFamilyTest" sheetId="50" r:id="rId42"/>
+    <sheet name="CorporateRegistrationTest" sheetId="51" r:id="rId43"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L4"/>
+  <oleSize ref="A1:J8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="376">
   <si>
     <t>TCID</t>
   </si>
@@ -541,21 +548,6 @@
     <t>08023138683</t>
   </si>
   <si>
-    <t>1543457</t>
-  </si>
-  <si>
-    <t>4147686936</t>
-  </si>
-  <si>
-    <t>myjona02</t>
-  </si>
-  <si>
-    <t>0032667536</t>
-  </si>
-  <si>
-    <t>ojojoguy03</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -823,36 +815,18 @@
     <t>TESTUSER1</t>
   </si>
   <si>
-    <t>samjo01</t>
-  </si>
-  <si>
     <t>Ebele</t>
   </si>
   <si>
-    <t>Amara</t>
-  </si>
-  <si>
     <t>selectUser</t>
   </si>
   <si>
     <t>Shasha</t>
   </si>
   <si>
-    <t>Melida</t>
-  </si>
-  <si>
     <t>saojo@systemspecs.com.ng</t>
   </si>
   <si>
-    <t>SAMJO01</t>
-  </si>
-  <si>
-    <t>samjo07</t>
-  </si>
-  <si>
-    <t>jombu07</t>
-  </si>
-  <si>
     <t>Ajala</t>
   </si>
   <si>
@@ -865,9 +839,6 @@
     <t>Biu</t>
   </si>
   <si>
-    <t>10977345</t>
-  </si>
-  <si>
     <t>nhfMonth</t>
   </si>
   <si>
@@ -901,9 +872,6 @@
     <t>S13342554</t>
   </si>
   <si>
-    <t>5006006296</t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
@@ -941,6 +909,282 @@
   </si>
   <si>
     <t>APP1</t>
+  </si>
+  <si>
+    <t>5006006298</t>
+  </si>
+  <si>
+    <t>5000.34</t>
+  </si>
+  <si>
+    <t>10978155</t>
+  </si>
+  <si>
+    <t>Johnbull</t>
+  </si>
+  <si>
+    <t>Alliyah</t>
+  </si>
+  <si>
+    <t>Aboh</t>
+  </si>
+  <si>
+    <t>benefitInst</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>benefitAcctNo</t>
+  </si>
+  <si>
+    <t>benefitName</t>
+  </si>
+  <si>
+    <t>Hajia Gambo</t>
+  </si>
+  <si>
+    <t>08023132768</t>
+  </si>
+  <si>
+    <t>384009</t>
+  </si>
+  <si>
+    <t>Kemisola Gambo</t>
+  </si>
+  <si>
+    <t>samson_ojo@yahoo.com</t>
+  </si>
+  <si>
+    <t>080376553354</t>
+  </si>
+  <si>
+    <t>Tel001</t>
+  </si>
+  <si>
+    <t>employerTIN</t>
+  </si>
+  <si>
+    <t>08034444555</t>
+  </si>
+  <si>
+    <t>1509322635633</t>
+  </si>
+  <si>
+    <t>employerCode</t>
+  </si>
+  <si>
+    <t>Josh-002</t>
+  </si>
+  <si>
+    <t>Joshua Jang</t>
+  </si>
+  <si>
+    <t>my address</t>
+  </si>
+  <si>
+    <t>tel-200</t>
+  </si>
+  <si>
+    <t>Jubril Emeka</t>
+  </si>
+  <si>
+    <t>08035467890</t>
+  </si>
+  <si>
+    <t>who2Pay</t>
+  </si>
+  <si>
+    <t>servicePurpose</t>
+  </si>
+  <si>
+    <t>payerAcctNo</t>
+  </si>
+  <si>
+    <t>1509323500888</t>
+  </si>
+  <si>
+    <t>Amadi John</t>
+  </si>
+  <si>
+    <t>08034323485</t>
+  </si>
+  <si>
+    <t>just another</t>
+  </si>
+  <si>
+    <t>08034898765</t>
+  </si>
+  <si>
+    <t>Jona Jega</t>
+  </si>
+  <si>
+    <t>08034542345</t>
+  </si>
+  <si>
+    <t>Komolafe Jubril</t>
+  </si>
+  <si>
+    <t>0067564345</t>
+  </si>
+  <si>
+    <t>corpID</t>
+  </si>
+  <si>
+    <t>cacRegNo</t>
+  </si>
+  <si>
+    <t>taxNo</t>
+  </si>
+  <si>
+    <t>introducedBy</t>
+  </si>
+  <si>
+    <t>corpName</t>
+  </si>
+  <si>
+    <t>institutionType</t>
+  </si>
+  <si>
+    <t>iniUserID</t>
+  </si>
+  <si>
+    <t>iniSurname</t>
+  </si>
+  <si>
+    <t>iniOthername</t>
+  </si>
+  <si>
+    <t>iniMobileNo</t>
+  </si>
+  <si>
+    <t>iniEmail</t>
+  </si>
+  <si>
+    <t>apprUserId</t>
+  </si>
+  <si>
+    <t>apprSurname</t>
+  </si>
+  <si>
+    <t>apprOthername</t>
+  </si>
+  <si>
+    <t>apprMobileNo</t>
+  </si>
+  <si>
+    <t>apprEmail</t>
+  </si>
+  <si>
+    <t>financialInst</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>transactionLimit</t>
+  </si>
+  <si>
+    <t>004637738</t>
+  </si>
+  <si>
+    <t>empPencomId</t>
+  </si>
+  <si>
+    <t>SYSP</t>
+  </si>
+  <si>
+    <t>HMOUPLOAD</t>
+  </si>
+  <si>
+    <t>24, Lewis Street, Lagos</t>
+  </si>
+  <si>
+    <t>Jubril</t>
+  </si>
+  <si>
+    <t>Komo</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Akpabio</t>
+  </si>
+  <si>
+    <t>10002</t>
+  </si>
+  <si>
+    <t>800000</t>
+  </si>
+  <si>
+    <t>qaremita@hot.com</t>
+  </si>
+  <si>
+    <t>08054376540</t>
+  </si>
+  <si>
+    <t>INIT007</t>
+  </si>
+  <si>
+    <t>APPR006</t>
+  </si>
+  <si>
+    <t>johncorp07</t>
+  </si>
+  <si>
+    <t>0044575649</t>
+  </si>
+  <si>
+    <t>0023546786</t>
+  </si>
+  <si>
+    <t>tel002</t>
+  </si>
+  <si>
+    <t>0076876544</t>
+  </si>
+  <si>
+    <t>063080780</t>
+  </si>
+  <si>
+    <t>Gbajabiamila Inc.</t>
+  </si>
+  <si>
+    <t>0243506363</t>
+  </si>
+  <si>
+    <t>JOMBU12</t>
+  </si>
+  <si>
+    <t>samjo10</t>
+  </si>
+  <si>
+    <t>samjo13</t>
+  </si>
+  <si>
+    <t>jombu13</t>
+  </si>
+  <si>
+    <t>1543459</t>
+  </si>
+  <si>
+    <t>4147686938</t>
+  </si>
+  <si>
+    <t>myjona04</t>
+  </si>
+  <si>
+    <t>0032667538</t>
+  </si>
+  <si>
+    <t>ojojoguy05</t>
+  </si>
+  <si>
+    <t>Try and pay up else your ward will be shoeless in no time</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1248,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -1015,6 +1259,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1751,7 +1996,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1776,7 +2021,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>375</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1936,7 +2181,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>27</v>
@@ -1955,7 +2200,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2007,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2189,7 +2434,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2209,11 +2454,11 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3">
-        <v>105</v>
+      <c r="A2" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2229,7 +2474,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2297,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2378,13 +2623,13 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
-        <v>163</v>
+        <v>370</v>
       </c>
       <c r="B2" t="s">
         <v>160</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>164</v>
+        <v>371</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>159</v>
@@ -2402,7 +2647,7 @@
         <v>144</v>
       </c>
       <c r="I2" t="s">
-        <v>165</v>
+        <v>372</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>161</v>
@@ -2411,7 +2656,7 @@
         <v>162</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>166</v>
+        <v>373</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>143</v>
@@ -2426,7 +2671,7 @@
         <v>153</v>
       </c>
       <c r="Q2" t="s">
-        <v>167</v>
+        <v>374</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>157</v>
@@ -2452,7 +2697,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2462,13 +2707,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>141</v>
@@ -2480,7 +2725,7 @@
         <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -2488,16 +2733,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>265</v>
+        <v>368</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
@@ -2506,7 +2751,7 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2514,16 +2759,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>369</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>20</v>
@@ -2552,7 +2797,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2562,13 +2807,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>141</v>
@@ -2585,16 +2830,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>367</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
@@ -2619,7 +2864,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2629,16 +2874,16 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -2647,7 +2892,7 @@
         <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -2655,25 +2900,25 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2733,154 +2978,154 @@
   <sheetData>
     <row r="1" spans="1:53">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="AW1" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>24</v>
@@ -2891,13 +3136,13 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>132</v>
@@ -2909,25 +3154,25 @@
         <v>92</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" t="s">
         <v>209</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="M2" t="s">
-        <v>214</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>132</v>
@@ -2936,10 +3181,10 @@
         <v>92</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>132</v>
@@ -2948,64 +3193,64 @@
         <v>132</v>
       </c>
       <c r="U2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="V2" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="W2" s="3" t="s">
+      <c r="AC2" t="s">
         <v>216</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="AD2" t="s">
         <v>217</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AF2" t="s">
         <v>219</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AC2" t="s">
-        <v>221</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AL2" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AN2" t="s">
         <v>226</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>231</v>
       </c>
       <c r="AO2" s="3" t="s">
         <v>132</v>
@@ -3014,25 +3259,25 @@
         <v>132</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="AR2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="AV2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="AX2" s="3" t="s">
         <v>105</v>
@@ -3068,10 +3313,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>90</v>
@@ -3091,13 +3336,13 @@
         <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>27</v>
@@ -3116,12 +3361,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3216,8 +3462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3285,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3318,19 +3564,19 @@
         <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3356,19 +3602,19 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="L2" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3380,8 +3626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3411,19 +3657,19 @@
         <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3449,13 +3695,13 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>119</v>
@@ -3464,7 +3710,7 @@
         <v>93</v>
       </c>
       <c r="L2" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3474,15 +3720,23 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3508,13 +3762,28 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -3539,10 +3808,25 @@
       <c r="H2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3559,7 +3843,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3580,10 +3864,10 @@
         <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -3591,7 +3875,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>66</v>
@@ -3600,10 +3884,10 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="E2" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -3612,6 +3896,250 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="H2" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>300</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2">
+        <v>8034437654</v>
+      </c>
+      <c r="E2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3660,6 +4188,519 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>30000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>361</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2">
+        <v>15000</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>271</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2">
+        <v>200900</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="I2" t="s">
+        <v>319</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="L2" t="s">
+        <v>271</v>
+      </c>
+      <c r="M2" t="s">
+        <v>317</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G2" t="s">
+        <v>347</v>
+      </c>
+      <c r="H2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="J2" t="s">
+        <v>348</v>
+      </c>
+      <c r="K2" t="s">
+        <v>349</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" t="s">
+        <v>357</v>
+      </c>
+      <c r="O2" t="s">
+        <v>350</v>
+      </c>
+      <c r="P2" t="s">
+        <v>351</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="X2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1"/>
+    <hyperlink ref="R2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
@@ -3686,7 +4727,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -3707,7 +4748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3729,7 +4770,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Adding Remita Demo Test
</commit_message>
<xml_diff>
--- a/bin/config/ePaymentConnector.xlsx
+++ b/bin/config/ePaymentConnector.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11220" windowHeight="3900" tabRatio="710" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="9450" windowHeight="2925" tabRatio="710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -52,12 +52,12 @@
     <sheet name="CorporateRegistrationTest" sheetId="51" r:id="rId43"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J8"/>
+  <oleSize ref="A1:I5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="375">
   <si>
     <t>TCID</t>
   </si>
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>OCHOGU</t>
-  </si>
-  <si>
-    <t>REMITA2</t>
   </si>
   <si>
     <t>amount</t>
@@ -2021,7 +2018,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2181,7 +2178,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>27</v>
@@ -2253,7 +2250,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2279,11 +2276,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
@@ -2444,10 +2441,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>24</v>
@@ -2455,10 +2452,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2561,61 +2558,61 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>24</v>
@@ -2623,58 +2620,58 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" t="s">
+        <v>371</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="K2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" t="s">
         <v>154</v>
       </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>373</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" t="s">
-        <v>372</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="N2" t="s">
-        <v>155</v>
-      </c>
-      <c r="O2" t="s">
-        <v>158</v>
-      </c>
-      <c r="P2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>374</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>30</v>
@@ -2707,25 +2704,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -2733,16 +2730,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
@@ -2751,7 +2748,7 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2759,16 +2756,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>20</v>
@@ -2807,22 +2804,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>24</v>
@@ -2830,16 +2827,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
@@ -2874,25 +2871,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -2900,25 +2897,25 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="D2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2978,154 +2975,154 @@
   <sheetData>
     <row r="1" spans="1:53">
       <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="AV1" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="AW1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>24</v>
@@ -3136,148 +3133,148 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" t="s">
         <v>245</v>
       </c>
-      <c r="C2" t="s">
-        <v>259</v>
-      </c>
-      <c r="D2" t="s">
-        <v>246</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>92</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" t="s">
         <v>208</v>
       </c>
-      <c r="M2" t="s">
-        <v>209</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>92</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="V2" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y2" t="s">
         <v>211</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" t="s">
         <v>215</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>216</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" t="s">
         <v>218</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AI2" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" t="s">
         <v>225</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="AR2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="AS2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT2" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" t="s">
         <v>230</v>
       </c>
-      <c r="AV2" t="s">
-        <v>231</v>
-      </c>
       <c r="AW2" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AX2" s="3" t="s">
         <v>105</v>
@@ -3313,10 +3310,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>90</v>
@@ -3336,13 +3333,13 @@
         <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" t="s">
         <v>262</v>
-      </c>
-      <c r="C2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D2" t="s">
-        <v>263</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>27</v>
@@ -3408,7 +3405,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3432,7 +3429,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
@@ -3564,19 +3561,19 @@
         <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3602,19 +3599,19 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L2" t="s">
         <v>273</v>
-      </c>
-      <c r="L2" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3657,19 +3654,19 @@
         <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3695,13 +3692,13 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>119</v>
@@ -3710,7 +3707,7 @@
         <v>93</v>
       </c>
       <c r="L2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3762,19 +3759,19 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>18</v>
@@ -3809,13 +3806,13 @@
         <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>119</v>
@@ -3864,10 +3861,10 @@
         <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -3875,7 +3872,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>66</v>
@@ -3884,10 +3881,10 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2" t="s">
         <v>280</v>
-      </c>
-      <c r="E2" t="s">
-        <v>281</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -3924,16 +3921,16 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -3942,7 +3939,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>52</v>
@@ -3957,7 +3954,7 @@
         <v>55</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>24</v>
@@ -3968,37 +3965,37 @@
         <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" t="s">
         <v>296</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M2" t="s">
         <v>4</v>
@@ -4034,7 +4031,7 @@
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>53</v>
@@ -4043,7 +4040,7 @@
         <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -4051,7 +4048,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>86</v>
@@ -4060,10 +4057,10 @@
         <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -4093,7 +4090,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -4105,10 +4102,10 @@
         <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>24</v>
@@ -4116,10 +4113,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" t="s">
         <v>305</v>
-      </c>
-      <c r="B2" t="s">
-        <v>306</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>66</v>
@@ -4128,10 +4125,10 @@
         <v>8034437654</v>
       </c>
       <c r="E2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" t="s">
         <v>307</v>
-      </c>
-      <c r="F2" t="s">
-        <v>308</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -4150,7 +4147,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4234,7 +4231,7 @@
         <v>98</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
@@ -4254,13 +4251,13 @@
         <v>30000</v>
       </c>
       <c r="E2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H2" t="s">
         <v>99</v>
@@ -4269,7 +4266,7 @@
         <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
@@ -4302,16 +4299,16 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>52</v>
@@ -4329,7 +4326,7 @@
         <v>98</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
@@ -4340,22 +4337,22 @@
         <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2">
         <v>15000</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>99</v>
@@ -4364,7 +4361,7 @@
         <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
@@ -4400,16 +4397,16 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -4421,7 +4418,7 @@
         <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>52</v>
@@ -4433,22 +4430,22 @@
         <v>54</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>7</v>
@@ -4462,43 +4459,43 @@
         <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G2">
         <v>200900</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>119</v>
@@ -4546,73 +4543,73 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
@@ -4620,37 +4617,37 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" t="s">
+        <v>346</v>
+      </c>
+      <c r="H2" t="s">
         <v>345</v>
       </c>
-      <c r="F2" t="s">
-        <v>364</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="J2" t="s">
         <v>347</v>
       </c>
-      <c r="H2" t="s">
-        <v>346</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>348</v>
-      </c>
-      <c r="K2" t="s">
-        <v>349</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
@@ -4659,34 +4656,34 @@
         <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O2" t="s">
+        <v>349</v>
+      </c>
+      <c r="P2" t="s">
         <v>350</v>
       </c>
-      <c r="P2" t="s">
-        <v>351</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S2" t="s">
         <v>29</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="X2" t="s">
         <v>4</v>
@@ -4727,7 +4724,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -4770,7 +4767,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -4835,7 +4832,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:J2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>